<commit_message>
Added tests for final uncovered lines--now 100%.
</commit_message>
<xml_diff>
--- a/test/eg_claimers_cases.xlsx
+++ b/test/eg_claimers_cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{197E7B1A-74BA-49E5-8654-F21C237D5C2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A56328F-CB40-42B1-B15D-D28B19410A09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28860" yWindow="120" windowWidth="28770" windowHeight="16170" xr2:uid="{EDC22AC3-0DEB-44A6-83ED-CB72A21F4428}"/>
+    <workbookView xWindow="4095" yWindow="675" windowWidth="24090" windowHeight="14790" xr2:uid="{EDC22AC3-0DEB-44A6-83ED-CB72A21F4428}"/>
   </bookViews>
   <sheets>
     <sheet name="end_game_cases" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="27">
   <si>
     <t>Board</t>
   </si>
@@ -110,6 +110,12 @@
     <t>pad</t>
   </si>
   <si>
+    <t>move unclaimed seeds off the board; seeds is sum of stores and owned children</t>
+  </si>
+  <si>
+    <t>DivvySeedsChildOnly</t>
+  </si>
+  <si>
     <r>
       <t>Divide unowned seeds and move to an owned child, remainder to lower count player, ignoring any unowned seeds (</t>
     </r>
@@ -121,7 +127,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>test oddity - store not reported</t>
+      <t>test oddity - seeds in store are ignored</t>
     </r>
     <r>
       <rPr>
@@ -133,12 +139,6 @@
       </rPr>
       <t>)</t>
     </r>
-  </si>
-  <si>
-    <t>move unclaimed seeds off the board; seeds is sum of stores and owned children</t>
-  </si>
-  <si>
-    <t>DivvySeedsChildOnly</t>
   </si>
 </sst>
 </file>
@@ -275,7 +275,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -303,6 +303,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -321,16 +325,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF9393"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -640,14 +651,14 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37DD2C51-94C0-49F6-B00F-C9310EAB31F5}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:BN17"/>
+  <dimension ref="A1:BN21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3570" ySplit="2880" topLeftCell="W4" activePane="bottomLeft"/>
+      <pane xSplit="3570" ySplit="2880" topLeftCell="AG4" activePane="bottomRight"/>
       <selection activeCell="BN3" sqref="BN3"/>
-      <selection pane="topRight" activeCell="AB1" sqref="AB1:AC1048576"/>
-      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
-      <selection pane="bottomRight" activeCell="AO5" sqref="AO5"/>
+      <selection pane="topRight" activeCell="AZ3" sqref="AZ3:BF3"/>
+      <selection pane="bottomLeft" activeCell="I19" sqref="I19"/>
+      <selection pane="bottomRight" activeCell="BB22" sqref="BB22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -655,29 +666,31 @@
     <col min="1" max="8" width="3.28515625" customWidth="1"/>
     <col min="9" max="9" width="4" customWidth="1"/>
     <col min="10" max="10" width="4" style="2" customWidth="1"/>
-    <col min="11" max="15" width="4" customWidth="1"/>
+    <col min="11" max="13" width="4" customWidth="1"/>
+    <col min="14" max="15" width="4" style="20" customWidth="1"/>
     <col min="16" max="16" width="6.28515625" style="7" customWidth="1"/>
     <col min="17" max="17" width="4" style="2" customWidth="1"/>
-    <col min="18" max="22" width="4" customWidth="1"/>
+    <col min="18" max="20" width="4" customWidth="1"/>
+    <col min="21" max="22" width="4" style="20" customWidth="1"/>
     <col min="23" max="23" width="6.28515625" style="5" customWidth="1"/>
     <col min="24" max="24" width="4" style="2" customWidth="1"/>
     <col min="25" max="27" width="4" customWidth="1"/>
-    <col min="28" max="29" width="4" style="26" customWidth="1"/>
+    <col min="28" max="29" width="4" style="20" customWidth="1"/>
     <col min="30" max="30" width="5.85546875" style="7" customWidth="1"/>
     <col min="31" max="34" width="4" customWidth="1"/>
-    <col min="35" max="36" width="4" style="26" customWidth="1"/>
+    <col min="35" max="36" width="4" style="20" customWidth="1"/>
     <col min="37" max="37" width="5.28515625" style="7" customWidth="1"/>
     <col min="38" max="41" width="4" customWidth="1"/>
-    <col min="42" max="43" width="4" style="26" customWidth="1"/>
+    <col min="42" max="43" width="4" style="20" customWidth="1"/>
     <col min="44" max="44" width="5.28515625" style="7" customWidth="1"/>
     <col min="45" max="48" width="4" customWidth="1"/>
-    <col min="49" max="50" width="4" style="26" customWidth="1"/>
+    <col min="49" max="50" width="4" style="20" customWidth="1"/>
     <col min="51" max="51" width="5.28515625" style="7" customWidth="1"/>
     <col min="52" max="55" width="4" customWidth="1"/>
-    <col min="56" max="57" width="4" style="26" customWidth="1"/>
+    <col min="56" max="57" width="4" style="20" customWidth="1"/>
     <col min="58" max="58" width="5.28515625" style="7" customWidth="1"/>
     <col min="59" max="62" width="4" customWidth="1"/>
-    <col min="63" max="64" width="4" style="26" customWidth="1"/>
+    <col min="63" max="64" width="4" style="20" customWidth="1"/>
     <col min="65" max="65" width="5.28515625" style="7" customWidth="1"/>
     <col min="66" max="83" width="4" customWidth="1"/>
   </cols>
@@ -686,46 +699,50 @@
       <c r="J1" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
       <c r="P1" s="6"/>
       <c r="Q1" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="U1" s="17"/>
+      <c r="V1" s="17"/>
       <c r="W1" s="3"/>
       <c r="X1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="AB1" s="23"/>
-      <c r="AC1" s="23"/>
+      <c r="AB1" s="17"/>
+      <c r="AC1" s="17"/>
       <c r="AD1" s="6"/>
       <c r="AE1" t="s">
         <v>10</v>
       </c>
-      <c r="AI1" s="23"/>
-      <c r="AJ1" s="23"/>
+      <c r="AI1" s="17"/>
+      <c r="AJ1" s="17"/>
       <c r="AK1" s="6"/>
       <c r="AL1" t="s">
         <v>14</v>
       </c>
-      <c r="AP1" s="23"/>
-      <c r="AQ1" s="23"/>
+      <c r="AP1" s="17"/>
+      <c r="AQ1" s="17"/>
       <c r="AR1" s="6"/>
       <c r="AS1" t="s">
         <v>11</v>
       </c>
-      <c r="AW1" s="23"/>
-      <c r="AX1" s="23"/>
+      <c r="AW1" s="17"/>
+      <c r="AX1" s="17"/>
       <c r="AY1" s="6"/>
       <c r="AZ1" t="s">
-        <v>26</v>
-      </c>
-      <c r="BD1" s="23"/>
-      <c r="BE1" s="23"/>
+        <v>25</v>
+      </c>
+      <c r="BD1" s="17"/>
+      <c r="BE1" s="17"/>
       <c r="BF1" s="6"/>
       <c r="BG1" t="s">
         <v>12</v>
       </c>
-      <c r="BK1" s="23"/>
-      <c r="BL1" s="23"/>
+      <c r="BK1" s="17"/>
+      <c r="BL1" s="17"/>
       <c r="BM1" s="6"/>
     </row>
     <row r="2" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -741,10 +758,10 @@
       <c r="J2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="N2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="O2" s="1" t="s">
+      <c r="N2" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O2" s="17" t="s">
         <v>3</v>
       </c>
       <c r="P2" s="6" t="s">
@@ -753,10 +770,10 @@
       <c r="Q2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="U2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="V2" s="1" t="s">
+      <c r="U2" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="V2" s="17" t="s">
         <v>3</v>
       </c>
       <c r="W2" s="3" t="s">
@@ -765,10 +782,10 @@
       <c r="X2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="AB2" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="AC2" s="23" t="s">
+      <c r="AB2" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC2" s="17" t="s">
         <v>3</v>
       </c>
       <c r="AD2" s="6" t="s">
@@ -777,10 +794,10 @@
       <c r="AE2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="AI2" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="AJ2" s="23" t="s">
+      <c r="AI2" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="AJ2" s="17" t="s">
         <v>3</v>
       </c>
       <c r="AK2" s="6" t="s">
@@ -789,10 +806,10 @@
       <c r="AL2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="AP2" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="AQ2" s="23" t="s">
+      <c r="AP2" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="AQ2" s="17" t="s">
         <v>3</v>
       </c>
       <c r="AR2" s="6" t="s">
@@ -801,10 +818,10 @@
       <c r="AS2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="AW2" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="AX2" s="23" t="s">
+      <c r="AW2" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="AX2" s="17" t="s">
         <v>3</v>
       </c>
       <c r="AY2" s="6" t="s">
@@ -813,10 +830,10 @@
       <c r="AZ2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="BD2" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="BE2" s="23" t="s">
+      <c r="BD2" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="BE2" s="17" t="s">
         <v>3</v>
       </c>
       <c r="BF2" s="6" t="s">
@@ -825,10 +842,10 @@
       <c r="BG2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="BK2" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="BL2" s="23" t="s">
+      <c r="BK2" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="BL2" s="17" t="s">
         <v>3</v>
       </c>
       <c r="BM2" s="6" t="s">
@@ -839,78 +856,78 @@
       </c>
     </row>
     <row r="3" spans="1:66" s="8" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J3" s="20" t="s">
+      <c r="J3" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="21"/>
-      <c r="N3" s="21"/>
-      <c r="O3" s="21"/>
-      <c r="P3" s="22"/>
-      <c r="Q3" s="20" t="s">
+      <c r="K3" s="25"/>
+      <c r="L3" s="25"/>
+      <c r="M3" s="25"/>
+      <c r="N3" s="25"/>
+      <c r="O3" s="25"/>
+      <c r="P3" s="26"/>
+      <c r="Q3" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="R3" s="21"/>
-      <c r="S3" s="21"/>
-      <c r="T3" s="21"/>
-      <c r="U3" s="21"/>
-      <c r="V3" s="21"/>
-      <c r="W3" s="22"/>
-      <c r="X3" s="20" t="s">
+      <c r="R3" s="25"/>
+      <c r="S3" s="25"/>
+      <c r="T3" s="25"/>
+      <c r="U3" s="25"/>
+      <c r="V3" s="25"/>
+      <c r="W3" s="26"/>
+      <c r="X3" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="Y3" s="21"/>
-      <c r="Z3" s="21"/>
-      <c r="AA3" s="21"/>
-      <c r="AB3" s="21"/>
-      <c r="AC3" s="21"/>
-      <c r="AD3" s="22"/>
-      <c r="AE3" s="17" t="s">
+      <c r="Y3" s="25"/>
+      <c r="Z3" s="25"/>
+      <c r="AA3" s="25"/>
+      <c r="AB3" s="25"/>
+      <c r="AC3" s="25"/>
+      <c r="AD3" s="26"/>
+      <c r="AE3" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="AF3" s="18"/>
-      <c r="AG3" s="18"/>
-      <c r="AH3" s="18"/>
-      <c r="AI3" s="18"/>
-      <c r="AJ3" s="18"/>
-      <c r="AK3" s="19"/>
-      <c r="AL3" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="AM3" s="18"/>
-      <c r="AN3" s="18"/>
-      <c r="AO3" s="18"/>
-      <c r="AP3" s="18"/>
-      <c r="AQ3" s="18"/>
-      <c r="AR3" s="19"/>
-      <c r="AS3" s="20" t="s">
+      <c r="AF3" s="22"/>
+      <c r="AG3" s="22"/>
+      <c r="AH3" s="22"/>
+      <c r="AI3" s="22"/>
+      <c r="AJ3" s="22"/>
+      <c r="AK3" s="23"/>
+      <c r="AL3" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="AM3" s="22"/>
+      <c r="AN3" s="22"/>
+      <c r="AO3" s="22"/>
+      <c r="AP3" s="22"/>
+      <c r="AQ3" s="22"/>
+      <c r="AR3" s="23"/>
+      <c r="AS3" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="AT3" s="21"/>
-      <c r="AU3" s="21"/>
-      <c r="AV3" s="21"/>
-      <c r="AW3" s="21"/>
-      <c r="AX3" s="21"/>
-      <c r="AY3" s="22"/>
-      <c r="AZ3" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="BA3" s="21"/>
-      <c r="BB3" s="21"/>
-      <c r="BC3" s="21"/>
-      <c r="BD3" s="21"/>
-      <c r="BE3" s="21"/>
-      <c r="BF3" s="22"/>
-      <c r="BG3" s="20" t="s">
+      <c r="AT3" s="25"/>
+      <c r="AU3" s="25"/>
+      <c r="AV3" s="25"/>
+      <c r="AW3" s="25"/>
+      <c r="AX3" s="25"/>
+      <c r="AY3" s="26"/>
+      <c r="AZ3" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="BA3" s="25"/>
+      <c r="BB3" s="25"/>
+      <c r="BC3" s="25"/>
+      <c r="BD3" s="25"/>
+      <c r="BE3" s="25"/>
+      <c r="BF3" s="26"/>
+      <c r="BG3" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="BH3" s="21"/>
-      <c r="BI3" s="21"/>
-      <c r="BJ3" s="21"/>
-      <c r="BK3" s="21"/>
-      <c r="BL3" s="21"/>
-      <c r="BM3" s="22"/>
+      <c r="BH3" s="25"/>
+      <c r="BI3" s="25"/>
+      <c r="BJ3" s="25"/>
+      <c r="BK3" s="25"/>
+      <c r="BL3" s="25"/>
+      <c r="BM3" s="26"/>
     </row>
     <row r="4" spans="1:66" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
@@ -940,10 +957,10 @@
       <c r="M4" s="9">
         <v>2</v>
       </c>
-      <c r="N4" s="9">
-        <v>0</v>
-      </c>
-      <c r="O4" s="9">
+      <c r="N4" s="18">
+        <v>0</v>
+      </c>
+      <c r="O4" s="18">
         <v>0</v>
       </c>
       <c r="P4" s="11" t="s">
@@ -961,10 +978,10 @@
       <c r="T4" s="9">
         <v>2</v>
       </c>
-      <c r="U4" s="9">
-        <v>0</v>
-      </c>
-      <c r="V4" s="9">
+      <c r="U4" s="18">
+        <v>0</v>
+      </c>
+      <c r="V4" s="18">
         <v>0</v>
       </c>
       <c r="W4" s="11" t="s">
@@ -982,10 +999,10 @@
       <c r="AA4" s="9">
         <v>2</v>
       </c>
-      <c r="AB4" s="24">
-        <v>0</v>
-      </c>
-      <c r="AC4" s="24">
+      <c r="AB4" s="18">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="18">
         <v>8</v>
       </c>
       <c r="AD4" s="11" t="s">
@@ -1003,10 +1020,10 @@
       <c r="AH4" s="9">
         <v>0</v>
       </c>
-      <c r="AI4" s="24">
+      <c r="AI4" s="18">
         <v>8</v>
       </c>
-      <c r="AJ4" s="24">
+      <c r="AJ4" s="18">
         <v>8</v>
       </c>
       <c r="AK4" s="11" t="s">
@@ -1024,10 +1041,10 @@
       <c r="AO4" s="9">
         <v>0</v>
       </c>
-      <c r="AP4" s="24">
-        <v>0</v>
-      </c>
-      <c r="AQ4" s="24">
+      <c r="AP4" s="18">
+        <v>0</v>
+      </c>
+      <c r="AQ4" s="18">
         <v>0</v>
       </c>
       <c r="AR4" s="11" t="s">
@@ -1045,10 +1062,10 @@
       <c r="AV4" s="9">
         <v>0</v>
       </c>
-      <c r="AW4" s="24">
+      <c r="AW4" s="18">
         <v>8</v>
       </c>
-      <c r="AX4" s="24">
+      <c r="AX4" s="18">
         <v>8</v>
       </c>
       <c r="AY4" s="11" t="s">
@@ -1066,10 +1083,10 @@
       <c r="BC4" s="9">
         <v>0</v>
       </c>
-      <c r="BD4" s="24">
-        <v>0</v>
-      </c>
-      <c r="BE4" s="24">
+      <c r="BD4" s="18">
+        <v>0</v>
+      </c>
+      <c r="BE4" s="18">
         <v>8</v>
       </c>
       <c r="BF4" s="11" t="s">
@@ -1087,10 +1104,10 @@
       <c r="BJ4" s="9">
         <v>2</v>
       </c>
-      <c r="BK4" s="24">
-        <v>0</v>
-      </c>
-      <c r="BL4" s="24">
+      <c r="BK4" s="18">
+        <v>0</v>
+      </c>
+      <c r="BL4" s="18">
         <v>8</v>
       </c>
       <c r="BM4" s="11" t="s">
@@ -1125,10 +1142,10 @@
       <c r="M5" s="12">
         <v>2</v>
       </c>
-      <c r="N5" s="12">
-        <v>0</v>
-      </c>
-      <c r="O5" s="12">
+      <c r="N5" s="19">
+        <v>0</v>
+      </c>
+      <c r="O5" s="19">
         <v>0</v>
       </c>
       <c r="P5" s="14"/>
@@ -1144,10 +1161,10 @@
       <c r="T5" s="12">
         <v>2</v>
       </c>
-      <c r="U5" s="12">
-        <v>0</v>
-      </c>
-      <c r="V5" s="12">
+      <c r="U5" s="19">
+        <v>0</v>
+      </c>
+      <c r="V5" s="19">
         <v>0</v>
       </c>
       <c r="W5" s="15"/>
@@ -1163,10 +1180,10 @@
       <c r="AA5" s="12">
         <v>2</v>
       </c>
-      <c r="AB5" s="25">
-        <v>0</v>
-      </c>
-      <c r="AC5" s="25">
+      <c r="AB5" s="19">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="19">
         <v>8</v>
       </c>
       <c r="AD5" s="14"/>
@@ -1182,10 +1199,10 @@
       <c r="AH5" s="12">
         <v>0</v>
       </c>
-      <c r="AI5" s="25">
+      <c r="AI5" s="19">
         <v>8</v>
       </c>
-      <c r="AJ5" s="25">
+      <c r="AJ5" s="19">
         <v>8</v>
       </c>
       <c r="AK5" s="14"/>
@@ -1201,10 +1218,10 @@
       <c r="AO5" s="12">
         <v>0</v>
       </c>
-      <c r="AP5" s="25">
-        <v>0</v>
-      </c>
-      <c r="AQ5" s="25">
+      <c r="AP5" s="19">
+        <v>0</v>
+      </c>
+      <c r="AQ5" s="19">
         <v>0</v>
       </c>
       <c r="AR5" s="14"/>
@@ -1220,10 +1237,10 @@
       <c r="AV5" s="12">
         <v>0</v>
       </c>
-      <c r="AW5" s="25">
+      <c r="AW5" s="19">
         <v>8</v>
       </c>
-      <c r="AX5" s="25">
+      <c r="AX5" s="19">
         <v>8</v>
       </c>
       <c r="AY5" s="14"/>
@@ -1239,10 +1256,10 @@
       <c r="BC5" s="12">
         <v>0</v>
       </c>
-      <c r="BD5" s="25">
-        <v>0</v>
-      </c>
-      <c r="BE5" s="25">
+      <c r="BD5" s="19">
+        <v>0</v>
+      </c>
+      <c r="BE5" s="19">
         <v>8</v>
       </c>
       <c r="BF5" s="14"/>
@@ -1258,10 +1275,10 @@
       <c r="BJ5" s="12">
         <v>2</v>
       </c>
-      <c r="BK5" s="25">
-        <v>0</v>
-      </c>
-      <c r="BL5" s="25">
+      <c r="BK5" s="19">
+        <v>0</v>
+      </c>
+      <c r="BL5" s="19">
         <v>8</v>
       </c>
       <c r="BM5" s="14"/>
@@ -1297,10 +1314,10 @@
       <c r="M6">
         <v>2</v>
       </c>
-      <c r="N6">
-        <v>1</v>
-      </c>
-      <c r="O6">
+      <c r="N6" s="20">
+        <v>1</v>
+      </c>
+      <c r="O6" s="20">
         <v>1</v>
       </c>
       <c r="P6" s="7" t="s">
@@ -1318,10 +1335,10 @@
       <c r="T6">
         <v>2</v>
       </c>
-      <c r="U6">
-        <v>1</v>
-      </c>
-      <c r="V6">
+      <c r="U6" s="20">
+        <v>1</v>
+      </c>
+      <c r="V6" s="20">
         <v>3</v>
       </c>
       <c r="W6" s="7" t="s">
@@ -1339,10 +1356,10 @@
       <c r="AA6">
         <v>2</v>
       </c>
-      <c r="AB6" s="26">
-        <v>1</v>
-      </c>
-      <c r="AC6" s="26">
+      <c r="AB6" s="20">
+        <v>1</v>
+      </c>
+      <c r="AC6" s="20">
         <v>7</v>
       </c>
       <c r="AD6" s="11" t="s">
@@ -1360,10 +1377,10 @@
       <c r="AH6">
         <v>0</v>
       </c>
-      <c r="AI6" s="26">
+      <c r="AI6" s="20">
         <v>5</v>
       </c>
-      <c r="AJ6" s="26">
+      <c r="AJ6" s="20">
         <v>7</v>
       </c>
       <c r="AK6" s="11" t="s">
@@ -1381,10 +1398,10 @@
       <c r="AO6">
         <v>0</v>
       </c>
-      <c r="AP6" s="26">
-        <v>1</v>
-      </c>
-      <c r="AQ6" s="26">
+      <c r="AP6" s="20">
+        <v>1</v>
+      </c>
+      <c r="AQ6" s="20">
         <v>3</v>
       </c>
       <c r="AR6" s="7" t="s">
@@ -1402,10 +1419,10 @@
       <c r="AV6">
         <v>0</v>
       </c>
-      <c r="AW6" s="26">
+      <c r="AW6" s="20">
         <v>5</v>
       </c>
-      <c r="AX6" s="26">
+      <c r="AX6" s="20">
         <v>7</v>
       </c>
       <c r="AY6" s="11" t="s">
@@ -1423,10 +1440,10 @@
       <c r="BC6">
         <v>0</v>
       </c>
-      <c r="BD6" s="26">
-        <v>1</v>
-      </c>
-      <c r="BE6" s="26">
+      <c r="BD6" s="20">
+        <v>1</v>
+      </c>
+      <c r="BE6" s="20">
         <v>6</v>
       </c>
       <c r="BF6" s="11" t="s">
@@ -1444,10 +1461,10 @@
       <c r="BJ6">
         <v>2</v>
       </c>
-      <c r="BK6" s="26">
-        <v>1</v>
-      </c>
-      <c r="BL6" s="26">
+      <c r="BK6" s="20">
+        <v>1</v>
+      </c>
+      <c r="BL6" s="20">
         <v>8</v>
       </c>
       <c r="BM6" s="7" t="s">
@@ -1485,10 +1502,10 @@
       <c r="M7" s="12">
         <v>1</v>
       </c>
-      <c r="N7" s="12">
-        <v>4</v>
-      </c>
-      <c r="O7" s="12">
+      <c r="N7" s="19">
+        <v>4</v>
+      </c>
+      <c r="O7" s="19">
         <v>4</v>
       </c>
       <c r="P7" s="14"/>
@@ -1504,10 +1521,10 @@
       <c r="T7" s="12">
         <v>1</v>
       </c>
-      <c r="U7" s="12">
-        <v>4</v>
-      </c>
-      <c r="V7" s="12">
+      <c r="U7" s="19">
+        <v>4</v>
+      </c>
+      <c r="V7" s="19">
         <v>6</v>
       </c>
       <c r="W7" s="15"/>
@@ -1523,10 +1540,10 @@
       <c r="AA7" s="12">
         <v>1</v>
       </c>
-      <c r="AB7" s="25">
-        <v>4</v>
-      </c>
-      <c r="AC7" s="25">
+      <c r="AB7" s="19">
+        <v>4</v>
+      </c>
+      <c r="AC7" s="19">
         <v>9</v>
       </c>
       <c r="AD7" s="14"/>
@@ -1542,10 +1559,10 @@
       <c r="AH7" s="12">
         <v>0</v>
       </c>
-      <c r="AI7" s="25">
+      <c r="AI7" s="19">
         <v>7</v>
       </c>
-      <c r="AJ7" s="25">
+      <c r="AJ7" s="19">
         <v>9</v>
       </c>
       <c r="AK7" s="14"/>
@@ -1561,10 +1578,10 @@
       <c r="AO7" s="12">
         <v>0</v>
       </c>
-      <c r="AP7" s="25">
-        <v>4</v>
-      </c>
-      <c r="AQ7" s="25">
+      <c r="AP7" s="19">
+        <v>4</v>
+      </c>
+      <c r="AQ7" s="19">
         <v>6</v>
       </c>
       <c r="AR7" s="14"/>
@@ -1580,10 +1597,10 @@
       <c r="AV7" s="12">
         <v>0</v>
       </c>
-      <c r="AW7" s="25">
+      <c r="AW7" s="19">
         <v>7</v>
       </c>
-      <c r="AX7" s="25">
+      <c r="AX7" s="19">
         <v>9</v>
       </c>
       <c r="AY7" s="14"/>
@@ -1599,10 +1616,10 @@
       <c r="BC7" s="12">
         <v>0</v>
       </c>
-      <c r="BD7" s="25">
-        <v>4</v>
-      </c>
-      <c r="BE7" s="25">
+      <c r="BD7" s="19">
+        <v>4</v>
+      </c>
+      <c r="BE7" s="19">
         <v>5</v>
       </c>
       <c r="BF7" s="14"/>
@@ -1618,10 +1635,10 @@
       <c r="BJ7" s="12">
         <v>1</v>
       </c>
-      <c r="BK7" s="25">
-        <v>4</v>
-      </c>
-      <c r="BL7" s="25">
+      <c r="BK7" s="19">
+        <v>4</v>
+      </c>
+      <c r="BL7" s="19">
         <v>8</v>
       </c>
       <c r="BM7" s="14"/>
@@ -1657,10 +1674,10 @@
       <c r="M8">
         <v>2</v>
       </c>
-      <c r="N8">
-        <v>2</v>
-      </c>
-      <c r="O8">
+      <c r="N8" s="20">
+        <v>2</v>
+      </c>
+      <c r="O8" s="20">
         <v>2</v>
       </c>
       <c r="P8" s="7" t="s">
@@ -1678,10 +1695,10 @@
       <c r="T8">
         <v>2</v>
       </c>
-      <c r="U8">
-        <v>2</v>
-      </c>
-      <c r="V8">
+      <c r="U8" s="20">
+        <v>2</v>
+      </c>
+      <c r="V8" s="20">
         <v>4</v>
       </c>
       <c r="W8" s="7" t="s">
@@ -1699,10 +1716,10 @@
       <c r="AA8">
         <v>2</v>
       </c>
-      <c r="AB8" s="26">
-        <v>2</v>
-      </c>
-      <c r="AC8" s="26">
+      <c r="AB8" s="20">
+        <v>2</v>
+      </c>
+      <c r="AC8" s="20">
         <v>7</v>
       </c>
       <c r="AD8" s="11" t="s">
@@ -1720,10 +1737,10 @@
       <c r="AH8">
         <v>0</v>
       </c>
-      <c r="AI8" s="26">
+      <c r="AI8" s="20">
         <v>5</v>
       </c>
-      <c r="AJ8" s="26">
+      <c r="AJ8" s="20">
         <v>7</v>
       </c>
       <c r="AK8" s="11" t="s">
@@ -1741,10 +1758,10 @@
       <c r="AO8">
         <v>0</v>
       </c>
-      <c r="AP8" s="26">
-        <v>2</v>
-      </c>
-      <c r="AQ8" s="26">
+      <c r="AP8" s="20">
+        <v>2</v>
+      </c>
+      <c r="AQ8" s="20">
         <v>4</v>
       </c>
       <c r="AR8" s="7" t="s">
@@ -1762,10 +1779,10 @@
       <c r="AV8">
         <v>0</v>
       </c>
-      <c r="AW8" s="26">
+      <c r="AW8" s="20">
         <v>5</v>
       </c>
-      <c r="AX8" s="26">
+      <c r="AX8" s="20">
         <v>7</v>
       </c>
       <c r="AY8" s="11" t="s">
@@ -1783,10 +1800,10 @@
       <c r="BC8">
         <v>0</v>
       </c>
-      <c r="BD8" s="26">
-        <v>2</v>
-      </c>
-      <c r="BE8" s="26">
+      <c r="BD8" s="20">
+        <v>2</v>
+      </c>
+      <c r="BE8" s="20">
         <v>5</v>
       </c>
       <c r="BF8" s="11" t="s">
@@ -1804,10 +1821,10 @@
       <c r="BJ8">
         <v>2</v>
       </c>
-      <c r="BK8" s="26">
-        <v>2</v>
-      </c>
-      <c r="BL8" s="26">
+      <c r="BK8" s="20">
+        <v>2</v>
+      </c>
+      <c r="BL8" s="20">
         <v>8</v>
       </c>
       <c r="BM8" s="7" t="s">
@@ -1845,10 +1862,10 @@
       <c r="M9">
         <v>1</v>
       </c>
-      <c r="N9">
-        <v>4</v>
-      </c>
-      <c r="O9">
+      <c r="N9" s="20">
+        <v>4</v>
+      </c>
+      <c r="O9" s="20">
         <v>4</v>
       </c>
       <c r="Q9" s="2">
@@ -1863,10 +1880,10 @@
       <c r="T9">
         <v>1</v>
       </c>
-      <c r="U9">
-        <v>4</v>
-      </c>
-      <c r="V9">
+      <c r="U9" s="20">
+        <v>4</v>
+      </c>
+      <c r="V9" s="20">
         <v>6</v>
       </c>
       <c r="X9" s="2">
@@ -1881,10 +1898,10 @@
       <c r="AA9">
         <v>1</v>
       </c>
-      <c r="AB9" s="26">
-        <v>4</v>
-      </c>
-      <c r="AC9" s="26">
+      <c r="AB9" s="20">
+        <v>4</v>
+      </c>
+      <c r="AC9" s="20">
         <v>9</v>
       </c>
       <c r="AE9" s="2">
@@ -1899,10 +1916,10 @@
       <c r="AH9">
         <v>0</v>
       </c>
-      <c r="AI9" s="26">
+      <c r="AI9" s="20">
         <v>7</v>
       </c>
-      <c r="AJ9" s="26">
+      <c r="AJ9" s="20">
         <v>9</v>
       </c>
       <c r="AL9">
@@ -1917,10 +1934,10 @@
       <c r="AO9">
         <v>0</v>
       </c>
-      <c r="AP9" s="26">
-        <v>4</v>
-      </c>
-      <c r="AQ9" s="26">
+      <c r="AP9" s="20">
+        <v>4</v>
+      </c>
+      <c r="AQ9" s="20">
         <v>6</v>
       </c>
       <c r="AS9" s="2">
@@ -1935,10 +1952,10 @@
       <c r="AV9">
         <v>0</v>
       </c>
-      <c r="AW9" s="26">
+      <c r="AW9" s="20">
         <v>7</v>
       </c>
-      <c r="AX9" s="26">
+      <c r="AX9" s="20">
         <v>9</v>
       </c>
       <c r="AZ9" s="2">
@@ -1953,10 +1970,10 @@
       <c r="BC9">
         <v>0</v>
       </c>
-      <c r="BD9" s="26">
-        <v>4</v>
-      </c>
-      <c r="BE9" s="26">
+      <c r="BD9" s="20">
+        <v>4</v>
+      </c>
+      <c r="BE9" s="20">
         <v>5</v>
       </c>
       <c r="BG9" s="2">
@@ -1971,10 +1988,10 @@
       <c r="BJ9">
         <v>1</v>
       </c>
-      <c r="BK9" s="26">
-        <v>4</v>
-      </c>
-      <c r="BL9" s="26">
+      <c r="BK9" s="20">
+        <v>4</v>
+      </c>
+      <c r="BL9" s="20">
         <v>8</v>
       </c>
     </row>
@@ -2009,10 +2026,10 @@
       <c r="M10" s="9">
         <v>1</v>
       </c>
-      <c r="N10" s="9">
-        <v>4</v>
-      </c>
-      <c r="O10" s="9">
+      <c r="N10" s="18">
+        <v>4</v>
+      </c>
+      <c r="O10" s="18">
         <v>4</v>
       </c>
       <c r="P10" s="11" t="s">
@@ -2030,10 +2047,10 @@
       <c r="T10" s="9">
         <v>1</v>
       </c>
-      <c r="U10" s="9">
-        <v>4</v>
-      </c>
-      <c r="V10" s="9">
+      <c r="U10" s="18">
+        <v>4</v>
+      </c>
+      <c r="V10" s="18">
         <v>6</v>
       </c>
       <c r="W10" s="16" t="s">
@@ -2051,10 +2068,10 @@
       <c r="AA10" s="9">
         <v>1</v>
       </c>
-      <c r="AB10" s="24">
-        <v>4</v>
-      </c>
-      <c r="AC10" s="24">
+      <c r="AB10" s="18">
+        <v>4</v>
+      </c>
+      <c r="AC10" s="18">
         <v>9</v>
       </c>
       <c r="AD10" s="11" t="s">
@@ -2072,10 +2089,10 @@
       <c r="AH10" s="9">
         <v>0</v>
       </c>
-      <c r="AI10" s="24">
+      <c r="AI10" s="18">
         <v>7</v>
       </c>
-      <c r="AJ10" s="24">
+      <c r="AJ10" s="18">
         <v>9</v>
       </c>
       <c r="AK10" s="11" t="s">
@@ -2093,10 +2110,10 @@
       <c r="AO10" s="9">
         <v>0</v>
       </c>
-      <c r="AP10" s="24">
-        <v>4</v>
-      </c>
-      <c r="AQ10" s="24">
+      <c r="AP10" s="18">
+        <v>4</v>
+      </c>
+      <c r="AQ10" s="18">
         <v>6</v>
       </c>
       <c r="AR10" s="11" t="s">
@@ -2114,10 +2131,10 @@
       <c r="AV10" s="9">
         <v>0</v>
       </c>
-      <c r="AW10" s="24">
+      <c r="AW10" s="18">
         <v>7</v>
       </c>
-      <c r="AX10" s="24">
+      <c r="AX10" s="18">
         <v>9</v>
       </c>
       <c r="AY10" s="11" t="s">
@@ -2135,10 +2152,10 @@
       <c r="BC10" s="9">
         <v>0</v>
       </c>
-      <c r="BD10" s="24">
-        <v>4</v>
-      </c>
-      <c r="BE10" s="24">
+      <c r="BD10" s="18">
+        <v>4</v>
+      </c>
+      <c r="BE10" s="18">
         <v>5</v>
       </c>
       <c r="BF10" s="11" t="s">
@@ -2156,10 +2173,10 @@
       <c r="BJ10" s="9">
         <v>1</v>
       </c>
-      <c r="BK10" s="24">
-        <v>4</v>
-      </c>
-      <c r="BL10" s="24">
+      <c r="BK10" s="18">
+        <v>4</v>
+      </c>
+      <c r="BL10" s="18">
         <v>8</v>
       </c>
       <c r="BM10" s="11" t="s">
@@ -2197,10 +2214,10 @@
       <c r="M11" s="12">
         <v>2</v>
       </c>
-      <c r="N11" s="12">
-        <v>2</v>
-      </c>
-      <c r="O11" s="12">
+      <c r="N11" s="19">
+        <v>2</v>
+      </c>
+      <c r="O11" s="19">
         <v>2</v>
       </c>
       <c r="P11" s="14"/>
@@ -2216,10 +2233,10 @@
       <c r="T11" s="12">
         <v>2</v>
       </c>
-      <c r="U11" s="12">
-        <v>2</v>
-      </c>
-      <c r="V11" s="12">
+      <c r="U11" s="19">
+        <v>2</v>
+      </c>
+      <c r="V11" s="19">
         <v>4</v>
       </c>
       <c r="W11" s="14"/>
@@ -2235,10 +2252,10 @@
       <c r="AA11" s="12">
         <v>2</v>
       </c>
-      <c r="AB11" s="25">
-        <v>2</v>
-      </c>
-      <c r="AC11" s="25">
+      <c r="AB11" s="19">
+        <v>2</v>
+      </c>
+      <c r="AC11" s="19">
         <v>7</v>
       </c>
       <c r="AD11" s="14"/>
@@ -2254,10 +2271,10 @@
       <c r="AH11" s="12">
         <v>0</v>
       </c>
-      <c r="AI11" s="25">
+      <c r="AI11" s="19">
         <v>5</v>
       </c>
-      <c r="AJ11" s="25">
+      <c r="AJ11" s="19">
         <v>7</v>
       </c>
       <c r="AK11" s="14"/>
@@ -2273,10 +2290,10 @@
       <c r="AO11" s="12">
         <v>0</v>
       </c>
-      <c r="AP11" s="25">
-        <v>2</v>
-      </c>
-      <c r="AQ11" s="25">
+      <c r="AP11" s="19">
+        <v>2</v>
+      </c>
+      <c r="AQ11" s="19">
         <v>4</v>
       </c>
       <c r="AR11" s="14"/>
@@ -2292,10 +2309,10 @@
       <c r="AV11" s="12">
         <v>0</v>
       </c>
-      <c r="AW11" s="25">
+      <c r="AW11" s="19">
         <v>5</v>
       </c>
-      <c r="AX11" s="25">
+      <c r="AX11" s="19">
         <v>7</v>
       </c>
       <c r="AY11" s="14"/>
@@ -2311,10 +2328,10 @@
       <c r="BC11" s="12">
         <v>0</v>
       </c>
-      <c r="BD11" s="25">
-        <v>2</v>
-      </c>
-      <c r="BE11" s="25">
+      <c r="BD11" s="19">
+        <v>2</v>
+      </c>
+      <c r="BE11" s="19">
         <v>5</v>
       </c>
       <c r="BF11" s="14"/>
@@ -2330,10 +2347,10 @@
       <c r="BJ11" s="12">
         <v>2</v>
       </c>
-      <c r="BK11" s="25">
-        <v>2</v>
-      </c>
-      <c r="BL11" s="25">
+      <c r="BK11" s="19">
+        <v>2</v>
+      </c>
+      <c r="BL11" s="19">
         <v>8</v>
       </c>
       <c r="BM11" s="14"/>
@@ -2369,10 +2386,10 @@
       <c r="M12">
         <v>2</v>
       </c>
-      <c r="N12">
-        <v>2</v>
-      </c>
-      <c r="O12">
+      <c r="N12" s="20">
+        <v>2</v>
+      </c>
+      <c r="O12" s="20">
         <v>2</v>
       </c>
       <c r="P12" s="7" t="s">
@@ -2390,10 +2407,10 @@
       <c r="T12">
         <v>2</v>
       </c>
-      <c r="U12">
-        <v>2</v>
-      </c>
-      <c r="V12">
+      <c r="U12" s="20">
+        <v>2</v>
+      </c>
+      <c r="V12" s="20">
         <v>4</v>
       </c>
       <c r="W12" s="7" t="s">
@@ -2411,10 +2428,10 @@
       <c r="AA12">
         <v>2</v>
       </c>
-      <c r="AB12" s="26">
-        <v>2</v>
-      </c>
-      <c r="AC12" s="26">
+      <c r="AB12" s="20">
+        <v>2</v>
+      </c>
+      <c r="AC12" s="20">
         <v>7</v>
       </c>
       <c r="AD12" s="11" t="s">
@@ -2432,10 +2449,10 @@
       <c r="AH12">
         <v>0</v>
       </c>
-      <c r="AI12" s="26">
+      <c r="AI12" s="20">
         <v>5</v>
       </c>
-      <c r="AJ12" s="26">
+      <c r="AJ12" s="20">
         <v>7</v>
       </c>
       <c r="AK12" s="11" t="s">
@@ -2453,10 +2470,10 @@
       <c r="AO12">
         <v>0</v>
       </c>
-      <c r="AP12" s="26">
-        <v>2</v>
-      </c>
-      <c r="AQ12" s="26">
+      <c r="AP12" s="20">
+        <v>2</v>
+      </c>
+      <c r="AQ12" s="20">
         <v>4</v>
       </c>
       <c r="AR12" s="7" t="s">
@@ -2474,10 +2491,10 @@
       <c r="AV12">
         <v>0</v>
       </c>
-      <c r="AW12" s="26">
-        <v>6</v>
-      </c>
-      <c r="AX12" s="26">
+      <c r="AW12" s="20">
+        <v>6</v>
+      </c>
+      <c r="AX12" s="20">
         <v>8</v>
       </c>
       <c r="AY12" s="11" t="s">
@@ -2495,10 +2512,10 @@
       <c r="BC12">
         <v>0</v>
       </c>
-      <c r="BD12" s="26">
-        <v>2</v>
-      </c>
-      <c r="BE12" s="26">
+      <c r="BD12" s="20">
+        <v>2</v>
+      </c>
+      <c r="BE12" s="20">
         <v>10</v>
       </c>
       <c r="BF12" s="11" t="s">
@@ -2516,10 +2533,10 @@
       <c r="BJ12">
         <v>2</v>
       </c>
-      <c r="BK12" s="26">
-        <v>2</v>
-      </c>
-      <c r="BL12" s="26">
+      <c r="BK12" s="20">
+        <v>2</v>
+      </c>
+      <c r="BL12" s="20">
         <v>8</v>
       </c>
       <c r="BM12" s="7" t="s">
@@ -2554,10 +2571,10 @@
       <c r="M13">
         <v>1</v>
       </c>
-      <c r="N13">
-        <v>4</v>
-      </c>
-      <c r="O13">
+      <c r="N13" s="20">
+        <v>4</v>
+      </c>
+      <c r="O13" s="20">
         <v>4</v>
       </c>
       <c r="Q13" s="2">
@@ -2572,10 +2589,10 @@
       <c r="T13">
         <v>1</v>
       </c>
-      <c r="U13">
-        <v>4</v>
-      </c>
-      <c r="V13">
+      <c r="U13" s="20">
+        <v>4</v>
+      </c>
+      <c r="V13" s="20">
         <v>4</v>
       </c>
       <c r="X13" s="2">
@@ -2590,10 +2607,10 @@
       <c r="AA13">
         <v>1</v>
       </c>
-      <c r="AB13" s="26">
-        <v>4</v>
-      </c>
-      <c r="AC13" s="26">
+      <c r="AB13" s="20">
+        <v>4</v>
+      </c>
+      <c r="AC13" s="20">
         <v>9</v>
       </c>
       <c r="AE13" s="2">
@@ -2608,10 +2625,10 @@
       <c r="AH13">
         <v>0</v>
       </c>
-      <c r="AI13" s="26">
+      <c r="AI13" s="20">
         <v>9</v>
       </c>
-      <c r="AJ13" s="26">
+      <c r="AJ13" s="20">
         <v>9</v>
       </c>
       <c r="AL13">
@@ -2626,10 +2643,10 @@
       <c r="AO13">
         <v>0</v>
       </c>
-      <c r="AP13" s="26">
-        <v>4</v>
-      </c>
-      <c r="AQ13" s="26">
+      <c r="AP13" s="20">
+        <v>4</v>
+      </c>
+      <c r="AQ13" s="20">
         <v>4</v>
       </c>
       <c r="AS13" s="2">
@@ -2644,10 +2661,10 @@
       <c r="AV13">
         <v>0</v>
       </c>
-      <c r="AW13" s="26">
+      <c r="AW13" s="20">
         <v>8</v>
       </c>
-      <c r="AX13" s="26">
+      <c r="AX13" s="20">
         <v>8</v>
       </c>
       <c r="AZ13" s="2">
@@ -2662,10 +2679,10 @@
       <c r="BC13">
         <v>0</v>
       </c>
-      <c r="BD13" s="26">
-        <v>4</v>
-      </c>
-      <c r="BE13" s="26">
+      <c r="BD13" s="20">
+        <v>4</v>
+      </c>
+      <c r="BE13" s="20">
         <v>0</v>
       </c>
       <c r="BG13" s="2">
@@ -2680,10 +2697,10 @@
       <c r="BJ13">
         <v>1</v>
       </c>
-      <c r="BK13" s="26">
-        <v>4</v>
-      </c>
-      <c r="BL13" s="26">
+      <c r="BK13" s="20">
+        <v>4</v>
+      </c>
+      <c r="BL13" s="20">
         <v>8</v>
       </c>
     </row>
@@ -2715,10 +2732,10 @@
       <c r="M14" s="9">
         <v>2</v>
       </c>
-      <c r="N14" s="9">
-        <v>2</v>
-      </c>
-      <c r="O14" s="9">
+      <c r="N14" s="18">
+        <v>2</v>
+      </c>
+      <c r="O14" s="18">
         <v>2</v>
       </c>
       <c r="P14" s="11" t="s">
@@ -2736,10 +2753,10 @@
       <c r="T14" s="9">
         <v>2</v>
       </c>
-      <c r="U14" s="9">
-        <v>2</v>
-      </c>
-      <c r="V14" s="9">
+      <c r="U14" s="18">
+        <v>2</v>
+      </c>
+      <c r="V14" s="18">
         <v>2</v>
       </c>
       <c r="W14" s="11" t="s">
@@ -2757,10 +2774,10 @@
       <c r="AA14" s="9">
         <v>2</v>
       </c>
-      <c r="AB14" s="24">
-        <v>2</v>
-      </c>
-      <c r="AC14" s="24">
+      <c r="AB14" s="18">
+        <v>2</v>
+      </c>
+      <c r="AC14" s="18">
         <v>7</v>
       </c>
       <c r="AD14" s="11" t="s">
@@ -2778,10 +2795,10 @@
       <c r="AH14" s="9">
         <v>0</v>
       </c>
-      <c r="AI14" s="24">
+      <c r="AI14" s="18">
         <v>7</v>
       </c>
-      <c r="AJ14" s="24">
+      <c r="AJ14" s="18">
         <v>7</v>
       </c>
       <c r="AK14" s="11" t="s">
@@ -2799,10 +2816,10 @@
       <c r="AO14" s="9">
         <v>0</v>
       </c>
-      <c r="AP14" s="24">
-        <v>2</v>
-      </c>
-      <c r="AQ14" s="24">
+      <c r="AP14" s="18">
+        <v>2</v>
+      </c>
+      <c r="AQ14" s="18">
         <v>2</v>
       </c>
       <c r="AR14" s="11" t="s">
@@ -2820,10 +2837,10 @@
       <c r="AV14" s="9">
         <v>0</v>
       </c>
-      <c r="AW14" s="24">
-        <v>6</v>
-      </c>
-      <c r="AX14" s="24">
+      <c r="AW14" s="18">
+        <v>6</v>
+      </c>
+      <c r="AX14" s="18">
         <v>6</v>
       </c>
       <c r="AY14" s="11" t="s">
@@ -2841,10 +2858,10 @@
       <c r="BC14" s="9">
         <v>0</v>
       </c>
-      <c r="BD14" s="24">
-        <v>2</v>
-      </c>
-      <c r="BE14" s="24">
+      <c r="BD14" s="18">
+        <v>2</v>
+      </c>
+      <c r="BE14" s="18">
         <v>0</v>
       </c>
       <c r="BF14" s="11" t="s">
@@ -2862,10 +2879,10 @@
       <c r="BJ14" s="9">
         <v>2</v>
       </c>
-      <c r="BK14" s="24">
-        <v>2</v>
-      </c>
-      <c r="BL14" s="24">
+      <c r="BK14" s="18">
+        <v>2</v>
+      </c>
+      <c r="BL14" s="18">
         <v>8</v>
       </c>
       <c r="BM14" s="11" t="s">
@@ -2903,10 +2920,10 @@
       <c r="M15" s="12">
         <v>1</v>
       </c>
-      <c r="N15" s="12">
-        <v>4</v>
-      </c>
-      <c r="O15" s="12">
+      <c r="N15" s="19">
+        <v>4</v>
+      </c>
+      <c r="O15" s="19">
         <v>4</v>
       </c>
       <c r="P15" s="14"/>
@@ -2922,10 +2939,10 @@
       <c r="T15" s="12">
         <v>1</v>
       </c>
-      <c r="U15" s="12">
-        <v>4</v>
-      </c>
-      <c r="V15" s="12">
+      <c r="U15" s="19">
+        <v>4</v>
+      </c>
+      <c r="V15" s="19">
         <v>6</v>
       </c>
       <c r="W15" s="15"/>
@@ -2941,10 +2958,10 @@
       <c r="AA15" s="12">
         <v>1</v>
       </c>
-      <c r="AB15" s="25">
-        <v>4</v>
-      </c>
-      <c r="AC15" s="25">
+      <c r="AB15" s="19">
+        <v>4</v>
+      </c>
+      <c r="AC15" s="19">
         <v>9</v>
       </c>
       <c r="AD15" s="14"/>
@@ -2960,10 +2977,10 @@
       <c r="AH15" s="12">
         <v>0</v>
       </c>
-      <c r="AI15" s="25">
+      <c r="AI15" s="19">
         <v>7</v>
       </c>
-      <c r="AJ15" s="25">
+      <c r="AJ15" s="19">
         <v>9</v>
       </c>
       <c r="AK15" s="14"/>
@@ -2979,10 +2996,10 @@
       <c r="AO15" s="12">
         <v>0</v>
       </c>
-      <c r="AP15" s="25">
-        <v>4</v>
-      </c>
-      <c r="AQ15" s="25">
+      <c r="AP15" s="19">
+        <v>4</v>
+      </c>
+      <c r="AQ15" s="19">
         <v>6</v>
       </c>
       <c r="AR15" s="14"/>
@@ -2998,10 +3015,10 @@
       <c r="AV15" s="12">
         <v>0</v>
       </c>
-      <c r="AW15" s="25">
+      <c r="AW15" s="19">
         <v>8</v>
       </c>
-      <c r="AX15" s="25">
+      <c r="AX15" s="19">
         <v>10</v>
       </c>
       <c r="AY15" s="14"/>
@@ -3017,10 +3034,10 @@
       <c r="BC15" s="12">
         <v>0</v>
       </c>
-      <c r="BD15" s="25">
-        <v>4</v>
-      </c>
-      <c r="BE15" s="25">
+      <c r="BD15" s="19">
+        <v>4</v>
+      </c>
+      <c r="BE15" s="19">
         <v>10</v>
       </c>
       <c r="BF15" s="14"/>
@@ -3036,10 +3053,10 @@
       <c r="BJ15" s="12">
         <v>1</v>
       </c>
-      <c r="BK15" s="25">
-        <v>4</v>
-      </c>
-      <c r="BL15" s="25">
+      <c r="BK15" s="19">
+        <v>4</v>
+      </c>
+      <c r="BL15" s="19">
         <v>8</v>
       </c>
       <c r="BM15" s="14"/>
@@ -3075,10 +3092,10 @@
       <c r="M16" s="9">
         <v>0</v>
       </c>
-      <c r="N16" s="9">
-        <v>6</v>
-      </c>
-      <c r="O16" s="9">
+      <c r="N16" s="18">
+        <v>6</v>
+      </c>
+      <c r="O16" s="18">
         <v>6</v>
       </c>
       <c r="P16" s="11" t="s">
@@ -3096,10 +3113,10 @@
       <c r="T16" s="9">
         <v>0</v>
       </c>
-      <c r="U16" s="9">
-        <v>6</v>
-      </c>
-      <c r="V16" s="9">
+      <c r="U16" s="18">
+        <v>6</v>
+      </c>
+      <c r="V16" s="18">
         <v>9</v>
       </c>
       <c r="W16" s="16" t="s">
@@ -3117,10 +3134,10 @@
       <c r="AA16" s="9">
         <v>0</v>
       </c>
-      <c r="AB16" s="24">
-        <v>6</v>
-      </c>
-      <c r="AC16" s="24">
+      <c r="AB16" s="18">
+        <v>6</v>
+      </c>
+      <c r="AC16" s="18">
         <v>9</v>
       </c>
       <c r="AD16" s="11" t="s">
@@ -3138,10 +3155,10 @@
       <c r="AH16" s="9">
         <v>0</v>
       </c>
-      <c r="AI16" s="24">
-        <v>6</v>
-      </c>
-      <c r="AJ16" s="24">
+      <c r="AI16" s="18">
+        <v>6</v>
+      </c>
+      <c r="AJ16" s="18">
         <v>9</v>
       </c>
       <c r="AK16" s="11" t="s">
@@ -3159,10 +3176,10 @@
       <c r="AO16" s="9">
         <v>0</v>
       </c>
-      <c r="AP16" s="24">
-        <v>6</v>
-      </c>
-      <c r="AQ16" s="24">
+      <c r="AP16" s="18">
+        <v>6</v>
+      </c>
+      <c r="AQ16" s="18">
         <v>9</v>
       </c>
       <c r="AR16" s="11" t="s">
@@ -3180,10 +3197,10 @@
       <c r="AV16" s="9">
         <v>0</v>
       </c>
-      <c r="AW16" s="24">
+      <c r="AW16" s="18">
         <v>7</v>
       </c>
-      <c r="AX16" s="24">
+      <c r="AX16" s="18">
         <v>10</v>
       </c>
       <c r="AY16" s="11" t="s">
@@ -3201,10 +3218,10 @@
       <c r="BC16" s="9">
         <v>0</v>
       </c>
-      <c r="BD16" s="24">
-        <v>6</v>
-      </c>
-      <c r="BE16" s="24">
+      <c r="BD16" s="18">
+        <v>6</v>
+      </c>
+      <c r="BE16" s="18">
         <v>4</v>
       </c>
       <c r="BF16" s="11" t="s">
@@ -3222,10 +3239,10 @@
       <c r="BJ16" s="9">
         <v>0</v>
       </c>
-      <c r="BK16" s="24">
-        <v>6</v>
-      </c>
-      <c r="BL16" s="24">
+      <c r="BK16" s="18">
+        <v>6</v>
+      </c>
+      <c r="BL16" s="18">
         <v>8</v>
       </c>
       <c r="BM16" s="11" t="s">
@@ -3263,10 +3280,10 @@
       <c r="M17" s="12">
         <v>2</v>
       </c>
-      <c r="N17" s="12">
-        <v>2</v>
-      </c>
-      <c r="O17" s="12">
+      <c r="N17" s="19">
+        <v>2</v>
+      </c>
+      <c r="O17" s="19">
         <v>2</v>
       </c>
       <c r="P17" s="14"/>
@@ -3282,10 +3299,10 @@
       <c r="T17" s="12">
         <v>2</v>
       </c>
-      <c r="U17" s="12">
-        <v>2</v>
-      </c>
-      <c r="V17" s="12">
+      <c r="U17" s="19">
+        <v>2</v>
+      </c>
+      <c r="V17" s="19">
         <v>4</v>
       </c>
       <c r="W17" s="14"/>
@@ -3301,10 +3318,10 @@
       <c r="AA17" s="12">
         <v>2</v>
       </c>
-      <c r="AB17" s="25">
-        <v>2</v>
-      </c>
-      <c r="AC17" s="25">
+      <c r="AB17" s="19">
+        <v>2</v>
+      </c>
+      <c r="AC17" s="19">
         <v>7</v>
       </c>
       <c r="AD17" s="14"/>
@@ -3320,10 +3337,10 @@
       <c r="AH17" s="12">
         <v>0</v>
       </c>
-      <c r="AI17" s="25">
+      <c r="AI17" s="19">
         <v>5</v>
       </c>
-      <c r="AJ17" s="25">
+      <c r="AJ17" s="19">
         <v>7</v>
       </c>
       <c r="AK17" s="14"/>
@@ -3339,10 +3356,10 @@
       <c r="AO17" s="12">
         <v>0</v>
       </c>
-      <c r="AP17" s="25">
-        <v>2</v>
-      </c>
-      <c r="AQ17" s="25">
+      <c r="AP17" s="19">
+        <v>2</v>
+      </c>
+      <c r="AQ17" s="19">
         <v>4</v>
       </c>
       <c r="AR17" s="14"/>
@@ -3358,10 +3375,10 @@
       <c r="AV17" s="12">
         <v>0</v>
       </c>
-      <c r="AW17" s="25">
-        <v>4</v>
-      </c>
-      <c r="AX17" s="25">
+      <c r="AW17" s="19">
+        <v>4</v>
+      </c>
+      <c r="AX17" s="19">
         <v>6</v>
       </c>
       <c r="AY17" s="14"/>
@@ -3377,10 +3394,10 @@
       <c r="BC17" s="12">
         <v>0</v>
       </c>
-      <c r="BD17" s="25">
-        <v>2</v>
-      </c>
-      <c r="BE17" s="25">
+      <c r="BD17" s="19">
+        <v>2</v>
+      </c>
+      <c r="BE17" s="19">
         <v>4</v>
       </c>
       <c r="BF17" s="14"/>
@@ -3396,13 +3413,387 @@
       <c r="BJ17" s="12">
         <v>2</v>
       </c>
-      <c r="BK17" s="25">
-        <v>2</v>
-      </c>
-      <c r="BL17" s="25">
+      <c r="BK17" s="19">
+        <v>2</v>
+      </c>
+      <c r="BL17" s="19">
         <v>8</v>
       </c>
       <c r="BM17" s="14"/>
+    </row>
+    <row r="18" spans="1:65" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="9">
+        <v>0</v>
+      </c>
+      <c r="B18" s="9">
+        <v>0</v>
+      </c>
+      <c r="C18" s="9">
+        <v>3</v>
+      </c>
+      <c r="D18" s="9">
+        <v>0</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I18" s="9">
+        <v>6</v>
+      </c>
+      <c r="J18" s="10">
+        <v>0</v>
+      </c>
+      <c r="K18" s="9">
+        <v>0</v>
+      </c>
+      <c r="L18" s="9">
+        <v>3</v>
+      </c>
+      <c r="M18" s="9">
+        <v>0</v>
+      </c>
+      <c r="N18" s="18">
+        <v>6</v>
+      </c>
+      <c r="O18" s="18">
+        <v>6</v>
+      </c>
+      <c r="P18" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q18" s="10">
+        <v>0</v>
+      </c>
+      <c r="R18" s="9">
+        <v>0</v>
+      </c>
+      <c r="S18" s="9">
+        <v>3</v>
+      </c>
+      <c r="T18" s="9">
+        <v>0</v>
+      </c>
+      <c r="U18" s="18">
+        <v>6</v>
+      </c>
+      <c r="V18" s="18">
+        <v>9</v>
+      </c>
+      <c r="W18" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="X18" s="10">
+        <v>0</v>
+      </c>
+      <c r="Y18" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="9">
+        <v>3</v>
+      </c>
+      <c r="AA18" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB18" s="18">
+        <v>6</v>
+      </c>
+      <c r="AC18" s="18">
+        <v>9</v>
+      </c>
+      <c r="AD18" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE18" s="10">
+        <v>0</v>
+      </c>
+      <c r="AF18" s="9">
+        <v>0</v>
+      </c>
+      <c r="AG18" s="9">
+        <v>3</v>
+      </c>
+      <c r="AH18" s="9">
+        <v>0</v>
+      </c>
+      <c r="AI18" s="18">
+        <v>6</v>
+      </c>
+      <c r="AJ18" s="18">
+        <v>9</v>
+      </c>
+      <c r="AK18" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="AL18" s="27">
+        <v>0</v>
+      </c>
+      <c r="AM18" s="27">
+        <v>0</v>
+      </c>
+      <c r="AN18" s="27">
+        <v>3</v>
+      </c>
+      <c r="AO18" s="27">
+        <v>0</v>
+      </c>
+      <c r="AP18" s="18">
+        <v>6</v>
+      </c>
+      <c r="AQ18" s="18">
+        <v>9</v>
+      </c>
+      <c r="AR18" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="AS18" s="10">
+        <v>0</v>
+      </c>
+      <c r="AT18" s="9">
+        <v>0</v>
+      </c>
+      <c r="AU18" s="9">
+        <v>3</v>
+      </c>
+      <c r="AV18" s="9">
+        <v>0</v>
+      </c>
+      <c r="AW18" s="18">
+        <v>6</v>
+      </c>
+      <c r="AX18" s="18">
+        <v>9</v>
+      </c>
+      <c r="AY18" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="AZ18" s="10">
+        <v>0</v>
+      </c>
+      <c r="BA18" s="9">
+        <v>0</v>
+      </c>
+      <c r="BB18" s="9">
+        <v>3</v>
+      </c>
+      <c r="BC18" s="9">
+        <v>0</v>
+      </c>
+      <c r="BD18" s="18">
+        <v>6</v>
+      </c>
+      <c r="BE18" s="18">
+        <v>3</v>
+      </c>
+      <c r="BF18" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="BG18" s="10">
+        <v>0</v>
+      </c>
+      <c r="BH18" s="9">
+        <v>0</v>
+      </c>
+      <c r="BI18" s="9">
+        <v>3</v>
+      </c>
+      <c r="BJ18" s="9">
+        <v>0</v>
+      </c>
+      <c r="BK18" s="18">
+        <v>6</v>
+      </c>
+      <c r="BL18" s="18">
+        <v>8</v>
+      </c>
+      <c r="BM18" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:65" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="12">
+        <v>1</v>
+      </c>
+      <c r="B19" s="12">
+        <v>2</v>
+      </c>
+      <c r="C19" s="12">
+        <v>0</v>
+      </c>
+      <c r="D19" s="12">
+        <v>2</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H19" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I19" s="12">
+        <v>2</v>
+      </c>
+      <c r="J19" s="13">
+        <v>1</v>
+      </c>
+      <c r="K19" s="12">
+        <v>2</v>
+      </c>
+      <c r="L19" s="12">
+        <v>0</v>
+      </c>
+      <c r="M19" s="12">
+        <v>2</v>
+      </c>
+      <c r="N19" s="19">
+        <v>2</v>
+      </c>
+      <c r="O19" s="19">
+        <v>2</v>
+      </c>
+      <c r="P19" s="14"/>
+      <c r="Q19" s="13">
+        <v>1</v>
+      </c>
+      <c r="R19" s="12">
+        <v>2</v>
+      </c>
+      <c r="S19" s="12">
+        <v>0</v>
+      </c>
+      <c r="T19" s="12">
+        <v>2</v>
+      </c>
+      <c r="U19" s="19">
+        <v>2</v>
+      </c>
+      <c r="V19" s="19">
+        <v>7</v>
+      </c>
+      <c r="W19" s="14"/>
+      <c r="X19" s="13">
+        <v>1</v>
+      </c>
+      <c r="Y19" s="12">
+        <v>2</v>
+      </c>
+      <c r="Z19" s="12">
+        <v>0</v>
+      </c>
+      <c r="AA19" s="12">
+        <v>2</v>
+      </c>
+      <c r="AB19" s="19">
+        <v>2</v>
+      </c>
+      <c r="AC19" s="19">
+        <v>7</v>
+      </c>
+      <c r="AD19" s="14"/>
+      <c r="AE19" s="13">
+        <v>1</v>
+      </c>
+      <c r="AF19" s="12">
+        <v>2</v>
+      </c>
+      <c r="AG19" s="12">
+        <v>0</v>
+      </c>
+      <c r="AH19" s="12">
+        <v>2</v>
+      </c>
+      <c r="AI19" s="19">
+        <v>2</v>
+      </c>
+      <c r="AJ19" s="19">
+        <v>7</v>
+      </c>
+      <c r="AK19" s="14"/>
+      <c r="AL19" s="28">
+        <v>1</v>
+      </c>
+      <c r="AM19" s="28">
+        <v>2</v>
+      </c>
+      <c r="AN19" s="28">
+        <v>0</v>
+      </c>
+      <c r="AO19" s="28">
+        <v>2</v>
+      </c>
+      <c r="AP19" s="19">
+        <v>2</v>
+      </c>
+      <c r="AQ19" s="19">
+        <v>7</v>
+      </c>
+      <c r="AR19" s="14"/>
+      <c r="AS19" s="13">
+        <v>1</v>
+      </c>
+      <c r="AT19" s="12">
+        <v>2</v>
+      </c>
+      <c r="AU19" s="12">
+        <v>0</v>
+      </c>
+      <c r="AV19" s="12">
+        <v>2</v>
+      </c>
+      <c r="AW19" s="19">
+        <v>2</v>
+      </c>
+      <c r="AX19" s="19">
+        <v>7</v>
+      </c>
+      <c r="AY19" s="14"/>
+      <c r="AZ19" s="13">
+        <v>1</v>
+      </c>
+      <c r="BA19" s="12">
+        <v>2</v>
+      </c>
+      <c r="BB19" s="12">
+        <v>0</v>
+      </c>
+      <c r="BC19" s="12">
+        <v>2</v>
+      </c>
+      <c r="BD19" s="19">
+        <v>2</v>
+      </c>
+      <c r="BE19" s="19">
+        <v>5</v>
+      </c>
+      <c r="BF19" s="14"/>
+      <c r="BG19" s="13">
+        <v>1</v>
+      </c>
+      <c r="BH19" s="12">
+        <v>2</v>
+      </c>
+      <c r="BI19" s="12">
+        <v>0</v>
+      </c>
+      <c r="BJ19" s="12">
+        <v>2</v>
+      </c>
+      <c r="BK19" s="19">
+        <v>2</v>
+      </c>
+      <c r="BL19" s="19">
+        <v>8</v>
+      </c>
+      <c r="BM19" s="14"/>
+    </row>
+    <row r="21" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="AM21" s="29"/>
+      <c r="AR21" s="30"/>
+      <c r="AS21" s="29"/>
+      <c r="AT21" s="29"/>
+      <c r="AU21" s="29"/>
+      <c r="BA21" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
Removed unused param to win_conditions. Removed the GAME_OVER WinCond--it is no longer needed. Removed win_count from game constants and mancala, it is now completely isolated to end_move. Streamlined the quitters--there was extra/unneeded code. Separated Winner into ClearWinner (near top of deco chain) and EndGameWinner (bottom of deco chain) Removed MaxWinner, it's functionality is now integrated into EndGameWinner. Removed the outcome assessment from NoOutcomeChange; and moved this in the deco chain to FIX a BUG!! Improved RoundWinner, it now translate a win/loss to round win/loss and detects round win/loss that are not apparent other ways. Olinda is behaving badly. First cut of test_cmp_end_move.py
</commit_message>
<xml_diff>
--- a/test/eg_claimers_cases.xlsx
+++ b/test/eg_claimers_cases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A56328F-CB40-42B1-B15D-D28B19410A09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10BE5052-8D88-4077-AA92-ED26C67B965A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4095" yWindow="675" windowWidth="24090" windowHeight="14790" xr2:uid="{EDC22AC3-0DEB-44A6-83ED-CB72A21F4428}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{EDC22AC3-0DEB-44A6-83ED-CB72A21F4428}"/>
   </bookViews>
   <sheets>
     <sheet name="end_game_cases" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="24">
   <si>
     <t>Board</t>
   </si>
@@ -74,16 +74,10 @@
     <t>DivvySeedsStores</t>
   </si>
   <si>
-    <t>DivvyIgnoreSeeds</t>
-  </si>
-  <si>
     <t>T</t>
   </si>
   <si>
     <t>TakeOnlyChildNStores</t>
-  </si>
-  <si>
-    <t xml:space="preserve">assert </t>
   </si>
   <si>
     <t>err</t>
@@ -102,9 +96,6 @@
   </si>
   <si>
     <t>Divide unowned seeds and move to store, remainder to lower count player, ignoring any unowned seeds</t>
-  </si>
-  <si>
-    <t>board &amp; store unchanged, ignore any seeds still in play; return win_count, win_count</t>
   </si>
   <si>
     <t>pad</t>
@@ -275,7 +266,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -307,6 +298,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -324,12 +318,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -651,10 +639,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37DD2C51-94C0-49F6-B00F-C9310EAB31F5}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:BN21"/>
+  <dimension ref="A1:BG21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3570" ySplit="2880" topLeftCell="AG4" activePane="bottomRight"/>
+      <pane xSplit="3570" ySplit="2880" topLeftCell="A4" activePane="topRight"/>
       <selection activeCell="BN3" sqref="BN3"/>
       <selection pane="topRight" activeCell="AZ3" sqref="AZ3:BF3"/>
       <selection pane="bottomLeft" activeCell="I19" sqref="I19"/>
@@ -689,13 +677,10 @@
     <col min="52" max="55" width="4" customWidth="1"/>
     <col min="56" max="57" width="4" style="20" customWidth="1"/>
     <col min="58" max="58" width="5.28515625" style="7" customWidth="1"/>
-    <col min="59" max="62" width="4" customWidth="1"/>
-    <col min="63" max="64" width="4" style="20" customWidth="1"/>
-    <col min="65" max="65" width="5.28515625" style="7" customWidth="1"/>
-    <col min="66" max="83" width="4" customWidth="1"/>
+    <col min="59" max="76" width="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:59" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="J1" s="2" t="s">
         <v>7</v>
       </c>
@@ -721,7 +706,7 @@
       <c r="AJ1" s="17"/>
       <c r="AK1" s="6"/>
       <c r="AL1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="AP1" s="17"/>
       <c r="AQ1" s="17"/>
@@ -733,19 +718,13 @@
       <c r="AX1" s="17"/>
       <c r="AY1" s="6"/>
       <c r="AZ1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="BD1" s="17"/>
       <c r="BE1" s="17"/>
       <c r="BF1" s="6"/>
-      <c r="BG1" t="s">
-        <v>12</v>
-      </c>
-      <c r="BK1" s="17"/>
-      <c r="BL1" s="17"/>
-      <c r="BM1" s="6"/>
     </row>
-    <row r="2" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:59" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -765,7 +744,7 @@
         <v>3</v>
       </c>
       <c r="P2" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="Q2" s="4" t="s">
         <v>5</v>
@@ -777,7 +756,7 @@
         <v>3</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="X2" s="4" t="s">
         <v>5</v>
@@ -789,7 +768,7 @@
         <v>3</v>
       </c>
       <c r="AD2" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="AE2" s="4" t="s">
         <v>5</v>
@@ -801,7 +780,7 @@
         <v>3</v>
       </c>
       <c r="AK2" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="AL2" s="1" t="s">
         <v>5</v>
@@ -813,7 +792,7 @@
         <v>3</v>
       </c>
       <c r="AR2" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="AS2" s="4" t="s">
         <v>5</v>
@@ -825,7 +804,7 @@
         <v>3</v>
       </c>
       <c r="AY2" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="AZ2" s="4" t="s">
         <v>5</v>
@@ -837,99 +816,78 @@
         <v>3</v>
       </c>
       <c r="BF2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="BG2" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:59" s="8" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J3" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="26"/>
+      <c r="N3" s="26"/>
+      <c r="O3" s="26"/>
+      <c r="P3" s="27"/>
+      <c r="Q3" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="BG2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="BK2" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="BL2" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="BM2" s="6" t="s">
+      <c r="R3" s="26"/>
+      <c r="S3" s="26"/>
+      <c r="T3" s="26"/>
+      <c r="U3" s="26"/>
+      <c r="V3" s="26"/>
+      <c r="W3" s="27"/>
+      <c r="X3" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="BN2" s="1" t="s">
+      <c r="Y3" s="26"/>
+      <c r="Z3" s="26"/>
+      <c r="AA3" s="26"/>
+      <c r="AB3" s="26"/>
+      <c r="AC3" s="26"/>
+      <c r="AD3" s="27"/>
+      <c r="AE3" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="AF3" s="23"/>
+      <c r="AG3" s="23"/>
+      <c r="AH3" s="23"/>
+      <c r="AI3" s="23"/>
+      <c r="AJ3" s="23"/>
+      <c r="AK3" s="24"/>
+      <c r="AL3" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="AM3" s="23"/>
+      <c r="AN3" s="23"/>
+      <c r="AO3" s="23"/>
+      <c r="AP3" s="23"/>
+      <c r="AQ3" s="23"/>
+      <c r="AR3" s="24"/>
+      <c r="AS3" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="AT3" s="26"/>
+      <c r="AU3" s="26"/>
+      <c r="AV3" s="26"/>
+      <c r="AW3" s="26"/>
+      <c r="AX3" s="26"/>
+      <c r="AY3" s="27"/>
+      <c r="AZ3" s="25" t="s">
         <v>23</v>
       </c>
+      <c r="BA3" s="26"/>
+      <c r="BB3" s="26"/>
+      <c r="BC3" s="26"/>
+      <c r="BD3" s="26"/>
+      <c r="BE3" s="26"/>
+      <c r="BF3" s="27"/>
     </row>
-    <row r="3" spans="1:66" s="8" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J3" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="25"/>
-      <c r="N3" s="25"/>
-      <c r="O3" s="25"/>
-      <c r="P3" s="26"/>
-      <c r="Q3" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="R3" s="25"/>
-      <c r="S3" s="25"/>
-      <c r="T3" s="25"/>
-      <c r="U3" s="25"/>
-      <c r="V3" s="25"/>
-      <c r="W3" s="26"/>
-      <c r="X3" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="Y3" s="25"/>
-      <c r="Z3" s="25"/>
-      <c r="AA3" s="25"/>
-      <c r="AB3" s="25"/>
-      <c r="AC3" s="25"/>
-      <c r="AD3" s="26"/>
-      <c r="AE3" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="AF3" s="22"/>
-      <c r="AG3" s="22"/>
-      <c r="AH3" s="22"/>
-      <c r="AI3" s="22"/>
-      <c r="AJ3" s="22"/>
-      <c r="AK3" s="23"/>
-      <c r="AL3" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="AM3" s="22"/>
-      <c r="AN3" s="22"/>
-      <c r="AO3" s="22"/>
-      <c r="AP3" s="22"/>
-      <c r="AQ3" s="22"/>
-      <c r="AR3" s="23"/>
-      <c r="AS3" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="AT3" s="25"/>
-      <c r="AU3" s="25"/>
-      <c r="AV3" s="25"/>
-      <c r="AW3" s="25"/>
-      <c r="AX3" s="25"/>
-      <c r="AY3" s="26"/>
-      <c r="AZ3" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="BA3" s="25"/>
-      <c r="BB3" s="25"/>
-      <c r="BC3" s="25"/>
-      <c r="BD3" s="25"/>
-      <c r="BE3" s="25"/>
-      <c r="BF3" s="26"/>
-      <c r="BG3" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="BH3" s="25"/>
-      <c r="BI3" s="25"/>
-      <c r="BJ3" s="25"/>
-      <c r="BK3" s="25"/>
-      <c r="BL3" s="25"/>
-      <c r="BM3" s="26"/>
-    </row>
-    <row r="4" spans="1:66" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:59" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>2</v>
       </c>
@@ -1048,7 +1006,7 @@
         <v>0</v>
       </c>
       <c r="AR4" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AS4" s="10">
         <v>0</v>
@@ -1090,31 +1048,10 @@
         <v>8</v>
       </c>
       <c r="BF4" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="BG4" s="10">
-        <v>2</v>
-      </c>
-      <c r="BH4" s="9">
-        <v>2</v>
-      </c>
-      <c r="BI4" s="9">
-        <v>2</v>
-      </c>
-      <c r="BJ4" s="9">
-        <v>2</v>
-      </c>
-      <c r="BK4" s="18">
-        <v>0</v>
-      </c>
-      <c r="BL4" s="18">
-        <v>8</v>
-      </c>
-      <c r="BM4" s="11" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:66" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:59" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <v>2</v>
       </c>
@@ -1263,27 +1200,8 @@
         <v>8</v>
       </c>
       <c r="BF5" s="14"/>
-      <c r="BG5" s="13">
-        <v>2</v>
-      </c>
-      <c r="BH5" s="12">
-        <v>2</v>
-      </c>
-      <c r="BI5" s="12">
-        <v>2</v>
-      </c>
-      <c r="BJ5" s="12">
-        <v>2</v>
-      </c>
-      <c r="BK5" s="19">
-        <v>0</v>
-      </c>
-      <c r="BL5" s="19">
-        <v>8</v>
-      </c>
-      <c r="BM5" s="14"/>
     </row>
-    <row r="6" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1297,7 +1215,7 @@
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I6">
         <v>1</v>
@@ -1405,7 +1323,7 @@
         <v>3</v>
       </c>
       <c r="AR6" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AS6" s="2">
         <v>0</v>
@@ -1449,29 +1367,8 @@
       <c r="BF6" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="BG6" s="2">
-        <v>2</v>
-      </c>
-      <c r="BH6">
-        <v>2</v>
-      </c>
-      <c r="BI6">
-        <v>0</v>
-      </c>
-      <c r="BJ6">
-        <v>2</v>
-      </c>
-      <c r="BK6" s="20">
-        <v>1</v>
-      </c>
-      <c r="BL6" s="20">
-        <v>8</v>
-      </c>
-      <c r="BM6" s="7" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="7" spans="1:66" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:59" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>2</v>
       </c>
@@ -1623,27 +1520,8 @@
         <v>5</v>
       </c>
       <c r="BF7" s="14"/>
-      <c r="BG7" s="13">
-        <v>2</v>
-      </c>
-      <c r="BH7" s="12">
-        <v>0</v>
-      </c>
-      <c r="BI7" s="12">
-        <v>2</v>
-      </c>
-      <c r="BJ7" s="12">
-        <v>1</v>
-      </c>
-      <c r="BK7" s="19">
-        <v>4</v>
-      </c>
-      <c r="BL7" s="19">
-        <v>8</v>
-      </c>
-      <c r="BM7" s="14"/>
     </row>
-    <row r="8" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1657,7 +1535,7 @@
         <v>2</v>
       </c>
       <c r="F8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I8">
         <v>2</v>
@@ -1765,7 +1643,7 @@
         <v>4</v>
       </c>
       <c r="AR8" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AS8" s="2">
         <v>0</v>
@@ -1809,29 +1687,8 @@
       <c r="BF8" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="BG8" s="2">
-        <v>1</v>
-      </c>
-      <c r="BH8">
-        <v>2</v>
-      </c>
-      <c r="BI8">
-        <v>0</v>
-      </c>
-      <c r="BJ8">
-        <v>2</v>
-      </c>
-      <c r="BK8" s="20">
-        <v>2</v>
-      </c>
-      <c r="BL8" s="20">
-        <v>8</v>
-      </c>
-      <c r="BM8" s="7" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="9" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
@@ -1976,26 +1833,8 @@
       <c r="BE9" s="20">
         <v>5</v>
       </c>
-      <c r="BG9" s="2">
-        <v>2</v>
-      </c>
-      <c r="BH9">
-        <v>0</v>
-      </c>
-      <c r="BI9">
-        <v>2</v>
-      </c>
-      <c r="BJ9">
-        <v>1</v>
-      </c>
-      <c r="BK9" s="20">
-        <v>4</v>
-      </c>
-      <c r="BL9" s="20">
-        <v>8</v>
-      </c>
     </row>
-    <row r="10" spans="1:66" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:59" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>2</v>
       </c>
@@ -2117,7 +1956,7 @@
         <v>6</v>
       </c>
       <c r="AR10" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AS10" s="10">
         <v>0</v>
@@ -2161,29 +2000,8 @@
       <c r="BF10" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="BG10" s="10">
-        <v>2</v>
-      </c>
-      <c r="BH10" s="9">
-        <v>0</v>
-      </c>
-      <c r="BI10" s="9">
-        <v>2</v>
-      </c>
-      <c r="BJ10" s="9">
-        <v>1</v>
-      </c>
-      <c r="BK10" s="18">
-        <v>4</v>
-      </c>
-      <c r="BL10" s="18">
-        <v>8</v>
-      </c>
-      <c r="BM10" s="11" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="11" spans="1:66" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:59" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <v>1</v>
       </c>
@@ -2197,7 +2015,7 @@
         <v>2</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I11" s="12">
         <v>2</v>
@@ -2335,27 +2153,8 @@
         <v>5</v>
       </c>
       <c r="BF11" s="14"/>
-      <c r="BG11" s="13">
-        <v>1</v>
-      </c>
-      <c r="BH11" s="12">
-        <v>2</v>
-      </c>
-      <c r="BI11" s="12">
-        <v>0</v>
-      </c>
-      <c r="BJ11" s="12">
-        <v>2</v>
-      </c>
-      <c r="BK11" s="19">
-        <v>2</v>
-      </c>
-      <c r="BL11" s="19">
-        <v>8</v>
-      </c>
-      <c r="BM11" s="14"/>
     </row>
-    <row r="12" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
@@ -2369,7 +2168,7 @@
         <v>2</v>
       </c>
       <c r="F12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I12">
         <v>2</v>
@@ -2477,7 +2276,7 @@
         <v>4</v>
       </c>
       <c r="AR12" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AS12" s="2">
         <v>0</v>
@@ -2521,29 +2320,8 @@
       <c r="BF12" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="BG12" s="2">
-        <v>1</v>
-      </c>
-      <c r="BH12">
-        <v>2</v>
-      </c>
-      <c r="BI12">
-        <v>0</v>
-      </c>
-      <c r="BJ12">
-        <v>2</v>
-      </c>
-      <c r="BK12" s="20">
-        <v>2</v>
-      </c>
-      <c r="BL12" s="20">
-        <v>8</v>
-      </c>
-      <c r="BM12" s="7" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="13" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2</v>
       </c>
@@ -2685,26 +2463,8 @@
       <c r="BE13" s="20">
         <v>0</v>
       </c>
-      <c r="BG13" s="2">
-        <v>2</v>
-      </c>
-      <c r="BH13">
-        <v>0</v>
-      </c>
-      <c r="BI13">
-        <v>2</v>
-      </c>
-      <c r="BJ13">
-        <v>1</v>
-      </c>
-      <c r="BK13" s="20">
-        <v>4</v>
-      </c>
-      <c r="BL13" s="20">
-        <v>8</v>
-      </c>
     </row>
-    <row r="14" spans="1:66" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:59" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>1</v>
       </c>
@@ -2823,7 +2583,7 @@
         <v>2</v>
       </c>
       <c r="AR14" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AS14" s="10">
         <v>0</v>
@@ -2867,29 +2627,8 @@
       <c r="BF14" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="BG14" s="10">
-        <v>1</v>
-      </c>
-      <c r="BH14" s="9">
-        <v>2</v>
-      </c>
-      <c r="BI14" s="9">
-        <v>0</v>
-      </c>
-      <c r="BJ14" s="9">
-        <v>2</v>
-      </c>
-      <c r="BK14" s="18">
-        <v>2</v>
-      </c>
-      <c r="BL14" s="18">
-        <v>8</v>
-      </c>
-      <c r="BM14" s="11" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="15" spans="1:66" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:59" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <v>2</v>
       </c>
@@ -3041,27 +2780,8 @@
         <v>10</v>
       </c>
       <c r="BF15" s="14"/>
-      <c r="BG15" s="13">
-        <v>2</v>
-      </c>
-      <c r="BH15" s="12">
-        <v>0</v>
-      </c>
-      <c r="BI15" s="12">
-        <v>2</v>
-      </c>
-      <c r="BJ15" s="12">
-        <v>1</v>
-      </c>
-      <c r="BK15" s="19">
-        <v>4</v>
-      </c>
-      <c r="BL15" s="19">
-        <v>8</v>
-      </c>
-      <c r="BM15" s="14"/>
     </row>
-    <row r="16" spans="1:66" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:59" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>0</v>
       </c>
@@ -3075,7 +2795,7 @@
         <v>0</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I16" s="9">
         <v>6</v>
@@ -3183,7 +2903,7 @@
         <v>9</v>
       </c>
       <c r="AR16" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AS16" s="10">
         <v>0</v>
@@ -3227,29 +2947,8 @@
       <c r="BF16" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="BG16" s="10">
-        <v>0</v>
-      </c>
-      <c r="BH16" s="9">
-        <v>0</v>
-      </c>
-      <c r="BI16" s="9">
-        <v>3</v>
-      </c>
-      <c r="BJ16" s="9">
-        <v>0</v>
-      </c>
-      <c r="BK16" s="18">
-        <v>6</v>
-      </c>
-      <c r="BL16" s="18">
-        <v>8</v>
-      </c>
-      <c r="BM16" s="11" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="17" spans="1:65" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:58" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <v>1</v>
       </c>
@@ -3401,27 +3100,8 @@
         <v>4</v>
       </c>
       <c r="BF17" s="14"/>
-      <c r="BG17" s="13">
-        <v>1</v>
-      </c>
-      <c r="BH17" s="12">
-        <v>2</v>
-      </c>
-      <c r="BI17" s="12">
-        <v>0</v>
-      </c>
-      <c r="BJ17" s="12">
-        <v>2</v>
-      </c>
-      <c r="BK17" s="19">
-        <v>2</v>
-      </c>
-      <c r="BL17" s="19">
-        <v>8</v>
-      </c>
-      <c r="BM17" s="14"/>
     </row>
-    <row r="18" spans="1:65" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:58" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <v>0</v>
       </c>
@@ -3435,7 +3115,7 @@
         <v>0</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I18" s="9">
         <v>6</v>
@@ -3524,16 +3204,16 @@
       <c r="AK18" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="AL18" s="27">
-        <v>0</v>
-      </c>
-      <c r="AM18" s="27">
-        <v>0</v>
-      </c>
-      <c r="AN18" s="27">
+      <c r="AL18" s="9">
+        <v>0</v>
+      </c>
+      <c r="AM18" s="9">
+        <v>0</v>
+      </c>
+      <c r="AN18" s="9">
         <v>3</v>
       </c>
-      <c r="AO18" s="27">
+      <c r="AO18" s="9">
         <v>0</v>
       </c>
       <c r="AP18" s="18">
@@ -3587,29 +3267,8 @@
       <c r="BF18" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="BG18" s="10">
-        <v>0</v>
-      </c>
-      <c r="BH18" s="9">
-        <v>0</v>
-      </c>
-      <c r="BI18" s="9">
-        <v>3</v>
-      </c>
-      <c r="BJ18" s="9">
-        <v>0</v>
-      </c>
-      <c r="BK18" s="18">
-        <v>6</v>
-      </c>
-      <c r="BL18" s="18">
-        <v>8</v>
-      </c>
-      <c r="BM18" s="11" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="19" spans="1:65" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:58" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
         <v>1</v>
       </c>
@@ -3710,16 +3369,16 @@
         <v>7</v>
       </c>
       <c r="AK19" s="14"/>
-      <c r="AL19" s="28">
-        <v>1</v>
-      </c>
-      <c r="AM19" s="28">
-        <v>2</v>
-      </c>
-      <c r="AN19" s="28">
-        <v>0</v>
-      </c>
-      <c r="AO19" s="28">
+      <c r="AL19" s="12">
+        <v>1</v>
+      </c>
+      <c r="AM19" s="12">
+        <v>2</v>
+      </c>
+      <c r="AN19" s="12">
+        <v>0</v>
+      </c>
+      <c r="AO19" s="12">
         <v>2</v>
       </c>
       <c r="AP19" s="19">
@@ -3767,40 +3426,15 @@
         <v>5</v>
       </c>
       <c r="BF19" s="14"/>
-      <c r="BG19" s="13">
-        <v>1</v>
-      </c>
-      <c r="BH19" s="12">
-        <v>2</v>
-      </c>
-      <c r="BI19" s="12">
-        <v>0</v>
-      </c>
-      <c r="BJ19" s="12">
-        <v>2</v>
-      </c>
-      <c r="BK19" s="19">
-        <v>2</v>
-      </c>
-      <c r="BL19" s="19">
-        <v>8</v>
-      </c>
-      <c r="BM19" s="14"/>
     </row>
-    <row r="21" spans="1:65" x14ac:dyDescent="0.25">
-      <c r="AM21" s="29"/>
-      <c r="AR21" s="30"/>
-      <c r="AS21" s="29"/>
-      <c r="AT21" s="29"/>
-      <c r="AU21" s="29"/>
-      <c r="BA21" s="29"/>
+    <row r="21" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="AR21" s="21"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="7">
     <mergeCell ref="AL3:AR3"/>
     <mergeCell ref="AS3:AY3"/>
     <mergeCell ref="AZ3:BF3"/>
-    <mergeCell ref="BG3:BM3"/>
     <mergeCell ref="J3:P3"/>
     <mergeCell ref="Q3:W3"/>
     <mergeCell ref="X3:AD3"/>

</xml_diff>